<commit_message>
draft submitted to committee
</commit_message>
<xml_diff>
--- a/future_directions_chapter/hbonding_toxgreen_data/finalReplicateData_with_ttests.xlsx
+++ b/future_directions_chapter/hbonding_toxgreen_data/finalReplicateData_with_ttests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Sequence-Design\CHIP2\gblocks\2024-3-24_gblockOrder\finalizedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3A852BAE-49DF-457B-A6FF-592D41365571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{810DDA31-B788-4073-A4AE-D4CC414317D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="4392" windowWidth="30936" windowHeight="16776" xr2:uid="{F28A2606-BCA6-4419-8859-A8EA49228C0A}"/>
+    <workbookView xWindow="45972" yWindow="3636" windowWidth="30936" windowHeight="16776" xr2:uid="{F28A2606-BCA6-4419-8859-A8EA49228C0A}"/>
   </bookViews>
   <sheets>
     <sheet name="t-tests" sheetId="2" r:id="rId1"/>
@@ -1238,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393F2E92-0303-40E5-AA18-609B77761F7E}">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>